<commit_message>
ASHRAE winter calibration example files
</commit_message>
<xml_diff>
--- a/projects/template_nsga.xlsx
+++ b/projects/template_nsga.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2374" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="747">
   <si>
     <t>type</t>
   </si>
@@ -1939,9 +1939,6 @@
   </si>
   <si>
     <t>integer</t>
-  </si>
-  <si>
-    <t>Temp</t>
   </si>
   <si>
     <t>Total Natural Gas Intensity</t>
@@ -5880,8 +5877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5919,7 +5916,7 @@
         <v>436</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>437</v>
@@ -5941,7 +5938,7 @@
         <v>471</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>616</v>
@@ -6013,28 +6010,28 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="24" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E9" s="24" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
         <v>$1.96/hour</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
+        <v>726</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>727</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>728</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6052,7 +6049,7 @@
         <v>39</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>473</v>
@@ -6063,7 +6060,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>617</v>
@@ -6099,7 +6096,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -6143,7 +6140,7 @@
         <v>453</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>545</v>
+        <v>553</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.3">
@@ -6172,138 +6169,142 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="23" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,1,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))=0,"",INDEX(Lookups!$C$21:$AC$30,1,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))</f>
-        <v>epsilonGradient</v>
+        <v>Number of Samples</v>
       </c>
       <c r="B25" s="18">
         <f>IF(D25&lt;&gt;"",D25,IF(LEN(INDEX(Lookups!$C$21:$AC$30,1,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1))=0,"",INDEX(Lookups!$C$21:$AC$30,1,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1)))</f>
-        <v>0.01</v>
+        <v>50</v>
       </c>
       <c r="C25" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,1,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))=0,"",INDEX(Lookups!$C$21:$AC$30,1,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))</f>
-        <v>epsilon in gradient calculation</v>
-      </c>
-      <c r="D25" s="27"/>
+        <v>Size of initial population</v>
+      </c>
+      <c r="D25" s="27">
+        <v>50</v>
+      </c>
       <c r="E25" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="23" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))=0,"",INDEX(Lookups!$C$21:$AC$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))</f>
-        <v>pgtol</v>
+        <v>Generations</v>
       </c>
       <c r="B26" s="18">
         <f>IF(D26&lt;&gt;"",D26,IF(LEN(INDEX(Lookups!$C$21:$AC$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1))=0,"",INDEX(Lookups!$C$21:$AC$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1)))</f>
-        <v>0.01</v>
+        <v>10</v>
       </c>
       <c r="C26" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))=0,"",INDEX(Lookups!$C$21:$AC$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))</f>
-        <v>tolerance on the projected gradient</v>
-      </c>
-      <c r="D26" s="27"/>
+        <v>Number of generations</v>
+      </c>
+      <c r="D26" s="27">
+        <v>10</v>
+      </c>
       <c r="E26" s="23"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="23" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,3,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))=0,"",INDEX(Lookups!$C$21:$AC$30,3,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))</f>
-        <v>factr</v>
+        <v>cprob</v>
       </c>
       <c r="B27" s="18">
         <f>IF(D27&lt;&gt;"",D27,IF(LEN(INDEX(Lookups!$C$21:$AC$30,3,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1))=0,"",INDEX(Lookups!$C$21:$AC$30,3,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1)))</f>
-        <v>45036000000000</v>
+        <v>0.85</v>
       </c>
       <c r="C27" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,3,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))=0,"",INDEX(Lookups!$C$21:$AC$30,3,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))</f>
-        <v>Tolerance on delta_F</v>
+        <v>Crossover probability [0,1]</v>
       </c>
       <c r="D27" s="27"/>
       <c r="E27" s="23"/>
     </row>
-    <row r="28" spans="1:6" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="23" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,4,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))=0,"",INDEX(Lookups!$C$21:$AC$30,4,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))</f>
-        <v>maxit</v>
+        <v>XoverDistIdx</v>
       </c>
       <c r="B28" s="18">
         <f>IF(D28&lt;&gt;"",D28,IF(LEN(INDEX(Lookups!$C$21:$AC$30,4,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1))=0,"",INDEX(Lookups!$C$21:$AC$30,4,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1)))</f>
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="C28" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,4,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))=0,"",INDEX(Lookups!$C$21:$AC$30,4,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))</f>
-        <v>Maximum number of iterations</v>
+        <v>Crossover Distribution Index (large values give higher probabilities of offspring close to parent)</v>
       </c>
       <c r="D28" s="27"/>
     </row>
-    <row r="29" spans="1:6" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="23" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,5,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))=0,"",INDEX(Lookups!$C$21:$AC$30,5,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))</f>
-        <v>normType</v>
-      </c>
-      <c r="B29" s="18" t="str">
+        <v>MuDistIdx</v>
+      </c>
+      <c r="B29" s="18">
         <f>IF(D29&lt;&gt;"",D29,IF(LEN(INDEX(Lookups!$C$21:$AC$30,5,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1))=0,"",INDEX(Lookups!$C$21:$AC$30,5,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1)))</f>
-        <v>minkowski</v>
+        <v>2</v>
       </c>
       <c r="C29" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,5,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))=0,"",INDEX(Lookups!$C$21:$AC$30,5,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))</f>
-        <v/>
+        <v>Mutation Distribution Index (large values give higher probabilities of offspring close to parent)</v>
       </c>
       <c r="D29" s="27"/>
     </row>
     <row r="30" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="23" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,6,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))=0,"",INDEX(Lookups!$C$21:$AC$30,6,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))</f>
-        <v>pPower</v>
+        <v>mprob</v>
       </c>
       <c r="B30" s="18">
         <f>IF(D30&lt;&gt;"",D30,IF(LEN(INDEX(Lookups!$C$21:$AC$30,6,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1))=0,"",INDEX(Lookups!$C$21:$AC$30,6,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1)))</f>
-        <v>2</v>
+        <v>0.8</v>
       </c>
       <c r="C30" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,6,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))=0,"",INDEX(Lookups!$C$21:$AC$30,6,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))</f>
-        <v>Lp norm power</v>
+        <v>Mutation probability [0,1]</v>
       </c>
       <c r="D30" s="27"/>
     </row>
     <row r="31" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="23" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,7,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))=0,"",INDEX(Lookups!$C$21:$AC$30,7,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))</f>
-        <v>Exit On Guideline14</v>
-      </c>
-      <c r="B31" s="18">
+        <v>normType</v>
+      </c>
+      <c r="B31" s="18" t="str">
         <f>IF(D31&lt;&gt;"",D31,IF(LEN(INDEX(Lookups!$C$21:$AC$30,7,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1))=0,"",INDEX(Lookups!$C$21:$AC$30,7,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1)))</f>
-        <v>0</v>
+        <v>minkowski</v>
       </c>
       <c r="C31" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,7,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))=0,"",INDEX(Lookups!$C$21:$AC$30,7,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))</f>
-        <v>0 false / 1 true (for use with calibration report)</v>
+        <v/>
       </c>
       <c r="D31" s="27"/>
     </row>
     <row r="32" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="23" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,8,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))=0,"",INDEX(Lookups!$C$21:$AC$30,8,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))</f>
-        <v/>
-      </c>
-      <c r="B32" s="18" t="str">
+        <v>pPower</v>
+      </c>
+      <c r="B32" s="18">
         <f>IF(D32&lt;&gt;"",D32,IF(LEN(INDEX(Lookups!$C$21:$AC$30,8,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1))=0,"",INDEX(Lookups!$C$21:$AC$30,8,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1)))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="C32" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,8,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))=0,"",INDEX(Lookups!$C$21:$AC$30,8,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))</f>
-        <v/>
+        <v>Lp norm power</v>
       </c>
       <c r="D32" s="27"/>
     </row>
     <row r="33" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="23" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,9,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))=0,"",INDEX(Lookups!$C$21:$AC$30,9,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-2))</f>
-        <v/>
-      </c>
-      <c r="B33" s="18" t="str">
+        <v>Exit On Guideline14</v>
+      </c>
+      <c r="B33" s="18">
         <f>IF(D33&lt;&gt;"",D33,IF(LEN(INDEX(Lookups!$C$21:$AC$30,9,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1))=0,"",INDEX(Lookups!$C$21:$AC$30,9,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)-1)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C33" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$AC$30,9,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))=0,"",INDEX(Lookups!$C$21:$AC$30,9,3*MATCH(Setup!$B22,Lookups!$A$21:$A$29,0)))</f>
-        <v/>
+        <v>0 false / 1 true (for use with calibration report)</v>
       </c>
       <c r="D33" s="27"/>
     </row>
@@ -6373,7 +6374,7 @@
         <v>29</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -6399,19 +6400,19 @@
         <v>32</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>35</v>
       </c>
@@ -6429,18 +6430,18 @@
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
+        <v>729</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>730</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="C46" s="6" t="s">
         <v>731</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>732</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="19"/>
       <c r="F46" s="8" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -6455,18 +6456,18 @@
     </row>
     <row r="49" spans="1:6" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
+        <v>733</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>734</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>735</v>
-      </c>
       <c r="C49" s="6" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="19"/>
       <c r="F49" s="8" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
   </sheetData>
@@ -6619,7 +6620,7 @@
         <v>36</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>11</v>
@@ -6765,7 +6766,7 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E6" s="42" t="s">
         <v>46</v>
@@ -7117,7 +7118,7 @@
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="42" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E15" s="42" t="s">
         <v>75</v>
@@ -7203,7 +7204,7 @@
       </c>
       <c r="C17" s="46"/>
       <c r="D17" s="46" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E17" s="46" t="s">
         <v>258</v>
@@ -7233,7 +7234,7 @@
       <c r="P17" s="42"/>
       <c r="Q17" s="42"/>
       <c r="R17" s="42" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="S17" s="42"/>
       <c r="T17" s="42"/>
@@ -7403,7 +7404,7 @@
       </c>
       <c r="C22" s="46"/>
       <c r="D22" s="46" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E22" s="46" t="s">
         <v>258</v>
@@ -7431,10 +7432,10 @@
       </c>
       <c r="O22" s="42"/>
       <c r="P22" s="42" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q22" s="42" t="s">
         <v>714</v>
-      </c>
-      <c r="Q22" s="42" t="s">
-        <v>715</v>
       </c>
       <c r="R22" s="42" t="s">
         <v>24</v>
@@ -7567,7 +7568,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C26" s="39" t="s">
         <v>76</v>
@@ -7607,7 +7608,7 @@
       </c>
       <c r="C27" s="46"/>
       <c r="D27" s="46" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E27" s="46" t="s">
         <v>77</v>
@@ -7731,7 +7732,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C30" s="39" t="s">
         <v>76</v>
@@ -7771,7 +7772,7 @@
       </c>
       <c r="C31" s="46"/>
       <c r="D31" s="46" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E31" s="46" t="s">
         <v>77</v>
@@ -7868,7 +7869,7 @@
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="10" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>84</v>
@@ -7935,13 +7936,13 @@
       </c>
       <c r="C35" s="42"/>
       <c r="D35" s="42" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E35" s="42" t="s">
         <v>172</v>
       </c>
       <c r="F35" s="42" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G35" s="42" t="s">
         <v>64</v>
@@ -8075,7 +8076,7 @@
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
       <c r="J38" s="15" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
@@ -9923,9 +9924,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9940,9 +9941,9 @@
     <col min="8" max="8" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.44140625" style="1" customWidth="1"/>
     <col min="14" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
@@ -9968,7 +9969,7 @@
         <v>461</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>620</v>
@@ -10007,7 +10008,7 @@
         <v>627</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C3" s="35" t="s">
         <v>628</v>
@@ -10037,22 +10038,20 @@
       <c r="L3" s="35" t="s">
         <v>632</v>
       </c>
-      <c r="M3" s="35" t="s">
-        <v>633</v>
-      </c>
+      <c r="M3" s="35"/>
     </row>
     <row r="4" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
+        <v>633</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>698</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>699</v>
-      </c>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>635</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>636</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>470</v>
@@ -10078,16 +10077,16 @@
     </row>
     <row r="5" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
+        <v>636</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>699</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>637</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>700</v>
-      </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="15" t="s">
         <v>638</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>639</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>470</v>
@@ -10107,21 +10106,23 @@
       <c r="J5" s="15">
         <v>590</v>
       </c>
-      <c r="K5" s="15"/>
+      <c r="K5" s="15">
+        <v>5</v>
+      </c>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
     </row>
     <row r="6" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>64</v>
@@ -10142,15 +10143,15 @@
     </row>
     <row r="7" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>64</v>
@@ -10171,15 +10172,15 @@
     </row>
     <row r="8" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>64</v>
@@ -10200,21 +10201,21 @@
     </row>
     <row r="9" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>64</v>
       </c>
       <c r="G9" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="15" t="b">
         <v>1</v>
@@ -10229,12 +10230,12 @@
     </row>
     <row r="10" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>470</v>
@@ -10258,12 +10259,12 @@
     </row>
     <row r="11" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>470</v>
@@ -10287,12 +10288,12 @@
     </row>
     <row r="12" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>470</v>
@@ -10316,12 +10317,12 @@
     </row>
     <row r="13" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>470</v>
@@ -10345,12 +10346,12 @@
     </row>
     <row r="14" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>470</v>
@@ -10374,12 +10375,12 @@
     </row>
     <row r="15" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>470</v>
@@ -10403,12 +10404,12 @@
     </row>
     <row r="16" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>470</v>
@@ -10432,12 +10433,12 @@
     </row>
     <row r="17" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>470</v>
@@ -10461,12 +10462,12 @@
     </row>
     <row r="18" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>470</v>
@@ -10490,12 +10491,12 @@
     </row>
     <row r="19" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>470</v>
@@ -10519,12 +10520,12 @@
     </row>
     <row r="20" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>470</v>
@@ -10548,12 +10549,12 @@
     </row>
     <row r="21" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>470</v>
@@ -10577,12 +10578,12 @@
     </row>
     <row r="22" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>470</v>
@@ -10606,12 +10607,12 @@
     </row>
     <row r="23" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>470</v>
@@ -10635,21 +10636,21 @@
     </row>
     <row r="24" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15" t="s">
+        <v>695</v>
+      </c>
+      <c r="E24" s="15" t="s">
         <v>696</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>697</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>64</v>
       </c>
       <c r="G24" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="15" t="b">
         <v>1</v>
@@ -19130,7 +19131,7 @@
         <v>439</v>
       </c>
       <c r="D1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -19138,19 +19139,19 @@
     </row>
     <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>643</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>644</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="22" t="s">
         <v>645</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>646</v>
-      </c>
       <c r="E2" s="22" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -19164,10 +19165,10 @@
         <v>594</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -19181,10 +19182,10 @@
         <v>596</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -19198,10 +19199,10 @@
         <v>598</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -19215,10 +19216,10 @@
         <v>600</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -19232,10 +19233,10 @@
         <v>602</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -19249,10 +19250,10 @@
         <v>603</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -19266,10 +19267,10 @@
         <v>605</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -19277,50 +19278,50 @@
         <v>606</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>607</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>446</v>
       </c>
       <c r="C11" s="22" t="s">
+        <v>722</v>
+      </c>
+      <c r="D11" s="22" t="s">
         <v>723</v>
       </c>
-      <c r="D11" s="22" t="s">
-        <v>724</v>
-      </c>
       <c r="E11" s="22" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>447</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -19391,10 +19392,10 @@
         <v>556</v>
       </c>
       <c r="X20" t="s">
+        <v>742</v>
+      </c>
+      <c r="AA20" t="s">
         <v>743</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
@@ -19438,7 +19439,7 @@
         <v>583</v>
       </c>
       <c r="AA21" s="22" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="AB21" s="22">
         <v>30</v>
@@ -19618,13 +19619,13 @@
         <v>556</v>
       </c>
       <c r="I27" s="22" t="s">
+        <v>745</v>
+      </c>
+      <c r="J27" s="23">
+        <v>0</v>
+      </c>
+      <c r="K27" s="23" t="s">
         <v>746</v>
-      </c>
-      <c r="J27" s="23">
-        <v>0</v>
-      </c>
-      <c r="K27" s="23" t="s">
-        <v>747</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>546</v>
@@ -19644,7 +19645,7 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>561</v>
@@ -19667,7 +19668,7 @@
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>562</v>
@@ -19679,13 +19680,13 @@
         <v>578</v>
       </c>
       <c r="O29" t="s">
+        <v>745</v>
+      </c>
+      <c r="P29" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="23" t="s">
         <v>746</v>
-      </c>
-      <c r="P29" s="23">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="23" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.3">
@@ -19709,13 +19710,13 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="L32" s="22" t="s">
+        <v>745</v>
+      </c>
+      <c r="M32" s="23">
+        <v>0</v>
+      </c>
+      <c r="N32" s="23" t="s">
         <v>746</v>
-      </c>
-      <c r="M32" s="23">
-        <v>0</v>
-      </c>
-      <c r="N32" s="23" t="s">
-        <v>747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>